<commit_message>
Ajuste LLD e HLD
</commit_message>
<xml_diff>
--- a/documentacao/Banco de Dados/Dicionário de dados.xlsx
+++ b/documentacao/Banco de Dados/Dicionário de dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\plant.ai\documentacao\Banco de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Plant.ai\documentacao\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -985,6 +985,105 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -993,121 +1092,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Estilo 1" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1329,8 +1320,8 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1347,19 +1338,19 @@
   <sheetData>
     <row r="1" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -1373,10 +1364,10 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1390,10 +1381,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1407,10 +1398,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1424,10 +1415,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1441,10 +1432,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -1461,37 +1452,37 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="28"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="28" t="s">
         <v>31</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -1515,12 +1506,12 @@
       <c r="M11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N11" s="29" t="s">
+      <c r="N11" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="11" t="s">
         <v>40</v>
       </c>
@@ -1562,7 +1553,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="11" t="s">
         <v>53</v>
       </c>
@@ -1604,7 +1595,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="11" t="s">
         <v>59</v>
       </c>
@@ -1646,7 +1637,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="37.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="11" t="s">
         <v>61</v>
       </c>
@@ -1688,41 +1679,41 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="113.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="32" t="s">
+      <c r="I16" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="K16" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="32" t="s">
+      <c r="L16" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="M16" s="32" t="s">
+      <c r="M16" s="27" t="s">
         <v>76</v>
       </c>
       <c r="N16" s="15" t="s">
@@ -1730,27 +1721,27 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="30"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="51"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="46"/>
     </row>
     <row r="19" spans="1:13" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="39" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1759,36 +1750,36 @@
       <c r="D19" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="47" t="s">
+      <c r="F19" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="47" t="s">
+      <c r="G19" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="47" t="s">
+      <c r="I19" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="J19" s="47" t="s">
+      <c r="J19" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="47" t="s">
+      <c r="K19" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="47" t="s">
+      <c r="L19" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="M19" s="48" t="s">
+      <c r="M19" s="41" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1821,12 +1812,12 @@
       <c r="L20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="M20" s="39" t="s">
+      <c r="M20" s="32" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="38" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1859,12 +1850,12 @@
       <c r="L21" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="M21" s="39" t="s">
+      <c r="M21" s="32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="39" t="s">
         <v>59</v>
       </c>
       <c r="C22" s="4">
@@ -1897,12 +1888,12 @@
       <c r="L22" s="4">
         <v>5</v>
       </c>
-      <c r="M22" s="39">
+      <c r="M22" s="32">
         <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1935,59 +1926,59 @@
       <c r="L23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M23" s="40"/>
+      <c r="M23" s="33"/>
     </row>
     <row r="24" spans="1:13" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="44" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="H24" s="32" t="s">
+      <c r="H24" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="I24" s="32" t="s">
+      <c r="I24" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="K24" s="32" t="s">
+      <c r="K24" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="L24" s="32" t="s">
+      <c r="L24" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="34" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="46"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -1997,19 +1988,19 @@
       <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:13" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="52" t="s">
+      <c r="F27" s="42" t="s">
         <v>117</v>
       </c>
       <c r="J27" s="8"/>
@@ -2018,7 +2009,7 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -2030,7 +2021,7 @@
       <c r="E28" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="33" t="s">
         <v>121</v>
       </c>
       <c r="J28" s="8"/>
@@ -2039,7 +2030,7 @@
       <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="38" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -2051,7 +2042,7 @@
       <c r="E29" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="33" t="s">
         <v>57</v>
       </c>
       <c r="J29" s="8"/>
@@ -2060,7 +2051,7 @@
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="38" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="4">
@@ -2072,7 +2063,7 @@
       <c r="E30" s="4">
         <v>1</v>
       </c>
-      <c r="F30" s="40">
+      <c r="F30" s="33">
         <v>3</v>
       </c>
       <c r="J30" s="8"/>
@@ -2081,7 +2072,7 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="39" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -2093,7 +2084,7 @@
       <c r="E31" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="33" t="s">
         <v>123</v>
       </c>
       <c r="J31" s="8"/>
@@ -2102,19 +2093,19 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" ht="94.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="41" t="s">
+      <c r="F32" s="34" t="s">
         <v>127</v>
       </c>
       <c r="J32" s="8"/>
@@ -2126,36 +2117,36 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="51"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="2:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="39" t="s">
         <v>27</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E35" s="47" t="s">
+      <c r="E35" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="F35" s="48" t="s">
+      <c r="F35" s="41" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -2167,12 +2158,12 @@
       <c r="E36" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F36" s="39" t="s">
+      <c r="F36" s="32" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="45" t="s">
+      <c r="B37" s="38" t="s">
         <v>53</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -2184,12 +2175,12 @@
       <c r="E37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="F37" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="39" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="4">
@@ -2201,12 +2192,12 @@
       <c r="E38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="39">
+      <c r="F38" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="36" t="s">
         <v>61</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -2218,24 +2209,24 @@
       <c r="E39" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="39" t="s">
+      <c r="F39" s="32" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="32" t="s">
+      <c r="D40" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="E40" s="32" t="s">
+      <c r="E40" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="F40" s="53" t="s">
+      <c r="F40" s="43" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>